<commit_message>
remove unnec col O
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2022.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2022.xlsx
@@ -158,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,13 +178,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -222,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -273,17 +266,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -314,31 +296,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -349,17 +329,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -575,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1000"/>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -587,10 +567,10 @@
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="12" width="8.7265625" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="26" width="8.7265625" customWidth="1"/>
+    <col min="14" max="23" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -598,9 +578,8 @@
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -615,2222 +594,1996 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="K3" s="8" t="s">
+      <c r="I3" s="8"/>
+      <c r="K3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="11"/>
-    </row>
-    <row r="4" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="9" t="s">
+    </row>
+    <row r="4" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="K4" s="9" t="s">
+      <c r="F4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="K4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9" t="s">
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="K5" s="9" t="s">
+      <c r="F5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="K5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="9"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="5"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="9"/>
+      <c r="K6" s="8"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="5"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13">
+    </row>
+    <row r="7" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
         <v>42430</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18">
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16">
         <v>42430</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="19" t="s">
+      <c r="J7" s="9"/>
+      <c r="K7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="16"/>
-    </row>
-    <row r="8" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="13">
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="12"/>
+    </row>
+    <row r="8" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
         <v>42431</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="20">
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="18">
         <v>42431</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="19" t="s">
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="17">
-        <f>6+(35/60)</f>
-        <v>6.583333333333333</v>
-      </c>
-      <c r="P8" s="21"/>
-    </row>
-    <row r="9" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="13">
+    </row>
+    <row r="9" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
         <v>42432</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="20">
+      <c r="D9" s="15"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="18">
         <v>42432</v>
       </c>
       <c r="J9" s="3"/>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="21"/>
-    </row>
-    <row r="10" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="13">
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="17"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
         <v>42433</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="20">
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="18">
         <v>42433</v>
       </c>
       <c r="J10" s="3"/>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="19" t="s">
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="17">
-        <f>6+(50/60)</f>
-        <v>6.833333333333333</v>
-      </c>
-      <c r="P10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="13">
+    </row>
+    <row r="11" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
         <v>42434</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="17" t="s">
+      <c r="D11" s="15"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="20">
         <f>7+(40/60)</f>
         <v>7.666666666666667</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="20">
+      <c r="H11" s="15"/>
+      <c r="I11" s="18">
         <v>42434</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="23" t="s">
+      <c r="J11" s="10"/>
+      <c r="K11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="19" t="s">
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="17">
-        <f>7+(40/60)</f>
-        <v>7.666666666666667</v>
-      </c>
-      <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="13">
+    </row>
+    <row r="12" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
         <v>42435</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="20">
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="18">
         <v>42435</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="19" t="s">
+      <c r="J12" s="10"/>
+      <c r="K12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="21"/>
-    </row>
-    <row r="13" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="13">
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="17"/>
+    </row>
+    <row r="13" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
         <v>42436</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="20">
+      <c r="D13" s="15"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="18">
         <v>42436</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="19" t="s">
+      <c r="J13" s="10"/>
+      <c r="K13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="19" t="s">
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="17">
-        <f>1+(20/60)</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="P13" s="21"/>
-    </row>
-    <row r="14" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="13">
+    </row>
+    <row r="14" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="11">
         <v>42437</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="11"/>
+      <c r="C14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="20">
+      <c r="D14" s="15"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="18">
         <v>42437</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="19" t="s">
+      <c r="J14" s="10"/>
+      <c r="K14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="19" t="s">
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="17">
-        <f>1+(45/60)</f>
-        <v>1.75</v>
-      </c>
-      <c r="P14" s="21"/>
-    </row>
-    <row r="15" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="13">
+    </row>
+    <row r="15" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="11">
         <v>42438</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="23" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="20">
+      <c r="D15" s="15"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="18">
         <v>42438</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="19" t="s">
+      <c r="J15" s="10"/>
+      <c r="K15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="19" t="s">
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="O15" s="17">
-        <f>2+(35/60)</f>
-        <v>2.5833333333333335</v>
-      </c>
-      <c r="P15" s="21"/>
-    </row>
-    <row r="16" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="13">
+    </row>
+    <row r="16" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
         <v>42439</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="23" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="20">
+      <c r="D16" s="15"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="18">
         <v>42439</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="19" t="s">
+      <c r="J16" s="10"/>
+      <c r="K16" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="19" t="s">
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="O16" s="17">
-        <f>7.5</f>
-        <v>7.5</v>
-      </c>
-      <c r="P16" s="21"/>
-    </row>
-    <row r="17" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="13">
+    </row>
+    <row r="17" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
         <v>42440</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="20">
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="18">
         <v>42440</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="19" t="s">
+      <c r="J17" s="10"/>
+      <c r="K17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="19" t="s">
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="O17" s="22">
+    </row>
+    <row r="18" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="11">
+        <v>42441</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="20">
         <v>4</v>
       </c>
-      <c r="P17" s="21"/>
-    </row>
-    <row r="18" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="13">
+      <c r="H18" s="15"/>
+      <c r="I18" s="18">
         <v>42441</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="19" t="s">
+      <c r="J18" s="10"/>
+      <c r="K18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="19" t="s">
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="22">
-        <v>4</v>
-      </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="20">
-        <v>42441</v>
-      </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="O18" s="22">
-        <v>4</v>
-      </c>
-      <c r="P18" s="21"/>
-    </row>
-    <row r="19" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="13">
+    </row>
+    <row r="19" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="11">
         <v>42442</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="20">
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="18">
         <v>42442</v>
       </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="17" t="s">
+      <c r="J19" s="10"/>
+      <c r="K19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="21"/>
-    </row>
-    <row r="20" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="13">
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="17"/>
+    </row>
+    <row r="20" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="11">
         <v>42443</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="19" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="20">
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="18">
         <v>42443</v>
       </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="19" t="s">
+      <c r="J20" s="10"/>
+      <c r="K20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="19" t="s">
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="17">
-        <f>15-7+(50/60)</f>
-        <v>8.8333333333333339</v>
-      </c>
-      <c r="P20" s="21"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13">
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="11">
         <v>42444</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26">
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="24">
         <v>42444</v>
       </c>
-      <c r="J21" s="27"/>
-      <c r="K21" s="28" t="s">
+      <c r="J21" s="25"/>
+      <c r="K21" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="28" t="s">
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="O21" s="17">
-        <f>16-7</f>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11">
+        <v>42445</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="18">
+        <v>42445</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="P21" s="21"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13">
-        <v>42445</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="19" t="s">
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="17"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11">
+        <v>42446</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="20">
-        <v>42445</v>
-      </c>
-      <c r="J22" s="12"/>
-      <c r="K22" s="19" t="s">
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="18">
+        <v>42446</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="21"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13">
-        <v>42446</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="19" t="s">
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="17"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="11">
+        <v>42447</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="20">
-        <v>42446</v>
-      </c>
-      <c r="J23" s="12"/>
-      <c r="K23" s="19" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="18">
+        <v>42447</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="21"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13">
-        <v>42447</v>
-      </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="20">
-        <v>42447</v>
-      </c>
-      <c r="J24" s="12"/>
-      <c r="K24" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="21"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13">
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="17"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="11">
         <v>42448</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="19" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="19" t="s">
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="15">
         <f>7+(10/60)</f>
         <v>7.166666666666667</v>
       </c>
-      <c r="H25" s="17"/>
-      <c r="I25" s="20">
+      <c r="H25" s="15"/>
+      <c r="I25" s="18">
         <v>42448</v>
       </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="19" t="s">
+      <c r="J25" s="15"/>
+      <c r="K25" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="19" t="s">
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="O25" s="17">
-        <f>18-11+(10/60)</f>
-        <v>7.166666666666667</v>
-      </c>
-      <c r="P25" s="21"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13">
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="11">
         <v>42449</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="19" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="20">
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="18">
         <v>42449</v>
       </c>
-      <c r="J26" s="17"/>
-      <c r="K26" s="19" t="s">
+      <c r="J26" s="15"/>
+      <c r="K26" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="21"/>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13">
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="17"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="11">
         <v>42450</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="23" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="20">
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="18">
         <v>42450</v>
       </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="19" t="s">
+      <c r="J27" s="15"/>
+      <c r="K27" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="21"/>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13">
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="17"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="11">
         <v>42451</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="19" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="20">
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="18">
         <v>42451</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="19" t="s">
+      <c r="J28" s="15"/>
+      <c r="K28" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="21"/>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13">
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="17"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="11">
         <v>42452</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="19" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="20">
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="18">
         <v>42452</v>
       </c>
-      <c r="J29" s="17"/>
-      <c r="K29" s="19" t="s">
+      <c r="J29" s="15"/>
+      <c r="K29" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="19" t="s">
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="O29" s="22">
-        <v>2</v>
-      </c>
-      <c r="P29" s="21"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13">
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="11">
         <v>42453</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="19" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="20">
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="18">
         <v>42453</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="19" t="s">
+      <c r="J30" s="15"/>
+      <c r="K30" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="19" t="s">
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="O30" s="22">
-        <v>3</v>
-      </c>
-      <c r="P30" s="21"/>
-    </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13">
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11">
         <v>42454</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="19" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="20">
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="18">
         <v>42454</v>
       </c>
-      <c r="J31" s="17"/>
-      <c r="K31" s="19" t="s">
+      <c r="J31" s="15"/>
+      <c r="K31" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="21"/>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13">
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="21"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11">
         <v>42455</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="19" t="s">
+      <c r="B32" s="11"/>
+      <c r="C32" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="20">
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="18">
         <v>42455</v>
       </c>
-      <c r="J32" s="17"/>
-      <c r="K32" s="19" t="s">
+      <c r="J32" s="15"/>
+      <c r="K32" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="21"/>
-    </row>
-    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13">
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="17"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11">
         <v>42456</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="19" t="s">
+      <c r="B33" s="11"/>
+      <c r="C33" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="20">
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="18">
         <v>42456</v>
       </c>
-      <c r="J33" s="17"/>
-      <c r="K33" s="19" t="s">
+      <c r="J33" s="15"/>
+      <c r="K33" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="L33" s="17"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="21"/>
-    </row>
-    <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="13">
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="17"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="11">
         <v>42457</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="23" t="s">
+      <c r="B34" s="11"/>
+      <c r="C34" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="20">
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="18">
         <v>42457</v>
       </c>
-      <c r="J34" s="17"/>
-      <c r="K34" s="19" t="s">
+      <c r="J34" s="15"/>
+      <c r="K34" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="19" t="s">
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="O34" s="22">
-        <v>10</v>
-      </c>
-      <c r="P34" s="21"/>
-    </row>
-    <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13">
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="11">
         <v>42458</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="23" t="s">
+      <c r="B35" s="11"/>
+      <c r="C35" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="20">
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="18">
         <v>42458</v>
       </c>
-      <c r="J35" s="17"/>
-      <c r="K35" s="19" t="s">
+      <c r="J35" s="15"/>
+      <c r="K35" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="23" t="s">
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O35" s="17">
-        <f>16-7+0.5</f>
-        <v>9.5</v>
-      </c>
-      <c r="P35" s="21"/>
-    </row>
-    <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="13">
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="11">
         <v>42459</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="19" t="s">
+      <c r="B36" s="11"/>
+      <c r="C36" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="20">
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="18">
         <v>42459</v>
       </c>
-      <c r="J36" s="17"/>
-      <c r="K36" s="19" t="s">
+      <c r="J36" s="15"/>
+      <c r="K36" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="21"/>
-    </row>
-    <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13">
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="21"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="11">
         <v>42460</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="19" t="s">
+      <c r="B37" s="11"/>
+      <c r="C37" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="20">
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="18">
         <v>42460</v>
       </c>
-      <c r="J37" s="17"/>
-      <c r="K37" s="19" t="s">
+      <c r="J37" s="15"/>
+      <c r="K37" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="21"/>
-    </row>
-    <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="13">
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="17"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11">
         <v>42461</v>
       </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="19" t="s">
+      <c r="B38" s="11"/>
+      <c r="C38" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="20">
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="18">
         <v>42461</v>
       </c>
-      <c r="J38" s="17"/>
-      <c r="K38" s="19" t="s">
+      <c r="J38" s="15"/>
+      <c r="K38" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="21"/>
-    </row>
-    <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13">
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="17"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="11">
         <v>42462</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="19" t="s">
+      <c r="B39" s="11"/>
+      <c r="C39" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="20">
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="18">
         <v>42462</v>
       </c>
-      <c r="J39" s="17"/>
-      <c r="K39" s="19" t="s">
+      <c r="J39" s="15"/>
+      <c r="K39" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="21"/>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13">
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="17"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="11">
         <v>42463</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="17" t="s">
+      <c r="B40" s="11"/>
+      <c r="C40" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="20">
+      <c r="E40" s="15"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="18">
         <v>42463</v>
       </c>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17" t="s">
+      <c r="J40" s="15"/>
+      <c r="K40" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="21"/>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13">
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="17"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="11">
         <v>42464</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="19" t="s">
+      <c r="B41" s="11"/>
+      <c r="C41" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="20">
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="18">
         <v>42464</v>
       </c>
-      <c r="J41" s="17"/>
-      <c r="K41" s="19" t="s">
+      <c r="J41" s="15"/>
+      <c r="K41" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="21"/>
-    </row>
-    <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13">
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="17"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="11">
         <v>42465</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="19" t="s">
+      <c r="B42" s="11"/>
+      <c r="C42" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="20">
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="18">
         <v>42465</v>
       </c>
-      <c r="J42" s="17"/>
-      <c r="K42" s="19" t="s">
+      <c r="J42" s="15"/>
+      <c r="K42" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="21"/>
-    </row>
-    <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="13">
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="17"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="11">
         <v>42466</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="19" t="s">
+      <c r="B43" s="11"/>
+      <c r="C43" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="20">
+      <c r="E43" s="15"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="18">
         <v>42466</v>
       </c>
-      <c r="J43" s="17"/>
-      <c r="K43" s="19" t="s">
+      <c r="J43" s="15"/>
+      <c r="K43" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="21"/>
-    </row>
-    <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="13">
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="17"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="11">
         <v>42467</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="19" t="s">
+      <c r="B44" s="11"/>
+      <c r="C44" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="20">
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="18">
         <v>42467</v>
       </c>
-      <c r="J44" s="17"/>
-      <c r="K44" s="19" t="s">
+      <c r="J44" s="15"/>
+      <c r="K44" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="21"/>
-    </row>
-    <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13">
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="17"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11">
         <v>42468</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="19" t="s">
+      <c r="B45" s="11"/>
+      <c r="C45" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="20">
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="18">
         <v>42468</v>
       </c>
-      <c r="J45" s="17"/>
-      <c r="K45" s="19" t="s">
+      <c r="J45" s="15"/>
+      <c r="K45" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L45" s="17"/>
-      <c r="M45" s="17"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="21"/>
-    </row>
-    <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13">
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="17"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="11">
         <v>42469</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="19" t="s">
+      <c r="B46" s="11"/>
+      <c r="C46" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="20">
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="18">
         <v>42469</v>
       </c>
-      <c r="J46" s="17"/>
-      <c r="K46" s="19" t="s">
+      <c r="J46" s="15"/>
+      <c r="K46" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="17"/>
-      <c r="P46" s="21"/>
-    </row>
-    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="13">
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="17"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="11">
         <v>42470</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="32" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="20">
+      <c r="E47" s="30"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="18">
         <v>42470</v>
       </c>
-      <c r="J47" s="17"/>
-      <c r="K47" s="32" t="s">
+      <c r="J47" s="15"/>
+      <c r="K47" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="L47" s="17"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="19"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="21"/>
-    </row>
-    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="13">
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="17"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="11">
         <v>42471</v>
       </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="19" t="s">
+      <c r="B48" s="11"/>
+      <c r="C48" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="20">
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="18">
         <v>42471</v>
       </c>
-      <c r="J48" s="17"/>
-      <c r="K48" s="19" t="s">
+      <c r="J48" s="15"/>
+      <c r="K48" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L48" s="17"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="19"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="21"/>
-    </row>
-    <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="13">
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="17"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="11">
         <v>42472</v>
       </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="19" t="s">
+      <c r="B49" s="11"/>
+      <c r="C49" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="20">
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="18">
         <v>42472</v>
       </c>
-      <c r="J49" s="17"/>
-      <c r="K49" s="19" t="s">
+      <c r="J49" s="15"/>
+      <c r="K49" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L49" s="17"/>
-      <c r="M49" s="17"/>
-      <c r="N49" s="19" t="s">
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="O49" s="22">
+    </row>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="11">
+        <v>42473</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="18">
+        <v>42473</v>
+      </c>
+      <c r="J50" s="15"/>
+      <c r="K50" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="11">
+        <v>42474</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="P49" s="21"/>
-    </row>
-    <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="13">
-        <v>42473</v>
-      </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="19" t="s">
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="18">
+        <v>42474</v>
+      </c>
+      <c r="J51" s="15"/>
+      <c r="K51" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="17"/>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="11">
+        <v>42475</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="18">
+        <v>42475</v>
+      </c>
+      <c r="J52" s="15"/>
+      <c r="K52" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
+      <c r="N52" s="17"/>
+    </row>
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="11">
+        <v>42476</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="18">
+        <v>42476</v>
+      </c>
+      <c r="J53" s="15"/>
+      <c r="K53" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="17"/>
+    </row>
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="11">
+        <v>42477</v>
+      </c>
+      <c r="B54" s="11"/>
+      <c r="C54" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="30"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="18">
+        <v>42477</v>
+      </c>
+      <c r="J54" s="15"/>
+      <c r="K54" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="17"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="11">
+        <v>42478</v>
+      </c>
+      <c r="B55" s="11"/>
+      <c r="C55" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="18">
+        <v>42478</v>
+      </c>
+      <c r="J55" s="15"/>
+      <c r="K55" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="17"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="11">
+        <v>42479</v>
+      </c>
+      <c r="B56" s="11"/>
+      <c r="C56" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="20">
-        <v>42473</v>
-      </c>
-      <c r="J50" s="17"/>
-      <c r="K50" s="23" t="s">
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="18">
+        <v>42479</v>
+      </c>
+      <c r="J56" s="15"/>
+      <c r="K56" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L50" s="17"/>
-      <c r="M50" s="17"/>
-      <c r="N50" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="O50" s="22">
-        <v>10</v>
-      </c>
-      <c r="P50" s="21"/>
-    </row>
-    <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="13">
-        <v>42474</v>
-      </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="19" t="s">
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="11">
+        <v>42480</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="18">
+        <v>42480</v>
+      </c>
+      <c r="J57" s="15"/>
+      <c r="K57" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="11">
+        <v>42481</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="18">
+        <v>42481</v>
+      </c>
+      <c r="J58" s="15"/>
+      <c r="K58" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="20">
-        <v>42474</v>
-      </c>
-      <c r="J51" s="17"/>
-      <c r="K51" s="19" t="s">
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="17"/>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="11">
+        <v>42482</v>
+      </c>
+      <c r="B59" s="11"/>
+      <c r="C59" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="18">
+        <v>42482</v>
+      </c>
+      <c r="J59" s="15"/>
+      <c r="K59" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L51" s="17"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="19"/>
-      <c r="O51" s="17"/>
-      <c r="P51" s="21"/>
-    </row>
-    <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="13">
-        <v>42475</v>
-      </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="19" t="s">
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="17"/>
+    </row>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="11">
+        <v>42483</v>
+      </c>
+      <c r="B60" s="11"/>
+      <c r="C60" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="20">
-        <v>42475</v>
-      </c>
-      <c r="J52" s="17"/>
-      <c r="K52" s="19" t="s">
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="18">
+        <v>42483</v>
+      </c>
+      <c r="J60" s="15"/>
+      <c r="K60" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L52" s="17"/>
-      <c r="M52" s="17"/>
-      <c r="N52" s="19"/>
-      <c r="O52" s="17"/>
-      <c r="P52" s="21"/>
-    </row>
-    <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="13">
-        <v>42476</v>
-      </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="19" t="s">
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="17"/>
+    </row>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="11">
+        <v>42484</v>
+      </c>
+      <c r="B61" s="11"/>
+      <c r="C61" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" s="30"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="18">
+        <v>42484</v>
+      </c>
+      <c r="J61" s="15"/>
+      <c r="K61" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="17"/>
+    </row>
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="11">
+        <v>42485</v>
+      </c>
+      <c r="B62" s="11"/>
+      <c r="C62" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="18">
+        <v>42485</v>
+      </c>
+      <c r="J62" s="15"/>
+      <c r="K62" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="11">
+        <v>42486</v>
+      </c>
+      <c r="B63" s="11"/>
+      <c r="C63" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="18">
+        <v>42486</v>
+      </c>
+      <c r="J63" s="10"/>
+      <c r="K63" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="11">
+        <v>42487</v>
+      </c>
+      <c r="B64" s="11"/>
+      <c r="C64" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="18">
+        <v>42487</v>
+      </c>
+      <c r="J64" s="10"/>
+      <c r="K64" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="11">
+        <v>42488</v>
+      </c>
+      <c r="B65" s="11"/>
+      <c r="C65" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="15"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="18">
+        <v>42488</v>
+      </c>
+      <c r="J65" s="10"/>
+      <c r="K65" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="20">
-        <v>42476</v>
-      </c>
-      <c r="J53" s="17"/>
-      <c r="K53" s="19" t="s">
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="21"/>
+    </row>
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="11">
+        <v>42489</v>
+      </c>
+      <c r="B66" s="22"/>
+      <c r="C66" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="15"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="18">
+        <v>42489</v>
+      </c>
+      <c r="J66" s="10"/>
+      <c r="K66" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="L53" s="17"/>
-      <c r="M53" s="17"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="17"/>
-      <c r="P53" s="21"/>
-    </row>
-    <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="13">
-        <v>42477</v>
-      </c>
-      <c r="B54" s="13"/>
-      <c r="C54" s="32" t="s">
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="17"/>
+    </row>
+    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="11">
+        <v>42490</v>
+      </c>
+      <c r="B67" s="22"/>
+      <c r="C67" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="11">
+        <v>42490</v>
+      </c>
+      <c r="J67" s="3"/>
+      <c r="K67" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L67" s="15"/>
+      <c r="M67" s="19"/>
+      <c r="N67" s="15"/>
+    </row>
+    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="11">
+        <v>43586</v>
+      </c>
+      <c r="B68" s="22"/>
+      <c r="C68" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="32"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="20">
-        <v>42477</v>
-      </c>
-      <c r="J54" s="17"/>
-      <c r="K54" s="32" t="s">
+      <c r="D68" s="15"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="11">
+        <v>43586</v>
+      </c>
+      <c r="J68" s="3"/>
+      <c r="K68" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="L54" s="17"/>
-      <c r="M54" s="17"/>
-      <c r="N54" s="19"/>
-      <c r="O54" s="17"/>
-      <c r="P54" s="21"/>
-    </row>
-    <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="13">
-        <v>42478</v>
-      </c>
-      <c r="B55" s="13"/>
-      <c r="C55" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="20">
-        <v>42478</v>
-      </c>
-      <c r="J55" s="17"/>
-      <c r="K55" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="19"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="21"/>
-    </row>
-    <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="13">
-        <v>42479</v>
-      </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="19" t="s">
+      <c r="L68" s="15"/>
+      <c r="M68" s="19"/>
+      <c r="N68" s="15"/>
+    </row>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="11">
+        <v>43587</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="20">
-        <v>42479</v>
-      </c>
-      <c r="J56" s="17"/>
-      <c r="K56" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="O56" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="P56" s="21"/>
-    </row>
-    <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="13">
-        <v>42480</v>
-      </c>
-      <c r="B57" s="13"/>
-      <c r="C57" s="19" t="s">
+      <c r="D69" s="15"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="18">
+        <v>43587</v>
+      </c>
+      <c r="J69" s="3"/>
+      <c r="K69" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L69" s="15"/>
+      <c r="M69" s="19"/>
+      <c r="N69" s="17"/>
+    </row>
+    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="18">
+        <v>43588</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="20">
-        <v>42480</v>
-      </c>
-      <c r="J57" s="17"/>
-      <c r="K57" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="L57" s="17"/>
-      <c r="M57" s="17"/>
-      <c r="N57" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="O57" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="P57" s="21"/>
-    </row>
-    <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="13">
-        <v>42481</v>
-      </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="19" t="s">
+      <c r="D70" s="15"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="19"/>
+      <c r="I70" s="18">
+        <v>43588</v>
+      </c>
+      <c r="J70" s="3"/>
+      <c r="K70" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L70" s="15"/>
+      <c r="M70" s="19"/>
+      <c r="N70" s="17"/>
+    </row>
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="18">
+        <v>43589</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="20">
-        <v>42481</v>
-      </c>
-      <c r="J58" s="17"/>
-      <c r="K58" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L58" s="17"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="19"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="21"/>
-    </row>
-    <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="13">
-        <v>42482</v>
-      </c>
-      <c r="B59" s="13"/>
-      <c r="C59" s="19" t="s">
+      <c r="D71" s="15"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="18">
+        <v>43589</v>
+      </c>
+      <c r="J71" s="3"/>
+      <c r="K71" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L71" s="15"/>
+      <c r="M71" s="19"/>
+      <c r="N71" s="17"/>
+    </row>
+    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="18">
+        <v>43590</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="20">
-        <v>42482</v>
-      </c>
-      <c r="J59" s="17"/>
-      <c r="K59" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L59" s="17"/>
-      <c r="M59" s="17"/>
-      <c r="N59" s="19"/>
-      <c r="O59" s="17"/>
-      <c r="P59" s="21"/>
-    </row>
-    <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="13">
-        <v>42483</v>
-      </c>
-      <c r="B60" s="13"/>
-      <c r="C60" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="20">
-        <v>42483</v>
-      </c>
-      <c r="J60" s="17"/>
-      <c r="K60" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L60" s="17"/>
-      <c r="M60" s="17"/>
-      <c r="N60" s="19"/>
-      <c r="O60" s="17"/>
-      <c r="P60" s="21"/>
-    </row>
-    <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="13">
-        <v>42484</v>
-      </c>
-      <c r="B61" s="13"/>
-      <c r="C61" s="32" t="s">
+      <c r="D72" s="15"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="18">
+        <v>43590</v>
+      </c>
+      <c r="J72" s="3"/>
+      <c r="K72" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L72" s="15"/>
+      <c r="M72" s="19"/>
+      <c r="N72" s="17"/>
+    </row>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="18">
+        <v>43591</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="18">
+        <v>43591</v>
+      </c>
+      <c r="J73" s="3"/>
+      <c r="K73" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L73" s="15"/>
+      <c r="M73" s="19"/>
+      <c r="N73" s="17"/>
+    </row>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="18">
+        <v>43592</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" s="15"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="18">
+        <v>43592</v>
+      </c>
+      <c r="J74" s="3"/>
+      <c r="K74" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L74" s="15"/>
+      <c r="M74" s="19"/>
+      <c r="N74" s="17"/>
+    </row>
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="18">
+        <v>43593</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="32"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="20">
-        <v>42484</v>
-      </c>
-      <c r="J61" s="17"/>
-      <c r="K61" s="32" t="s">
+      <c r="D75" s="15"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="18">
+        <v>43593</v>
+      </c>
+      <c r="J75" s="3"/>
+      <c r="K75" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="L61" s="17"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="19"/>
-      <c r="O61" s="17"/>
-      <c r="P61" s="21"/>
-    </row>
-    <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="13">
-        <v>42485</v>
-      </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="19" t="s">
+      <c r="L75" s="15"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="17"/>
+    </row>
+    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="18">
+        <v>43594</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="20">
-        <v>42485</v>
-      </c>
-      <c r="J62" s="17"/>
-      <c r="K62" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="L62" s="17"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="O62" s="22">
-        <v>8.3333300000000001</v>
-      </c>
-      <c r="P62" s="21"/>
-    </row>
-    <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="13">
-        <v>42486</v>
-      </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="19" t="s">
+      <c r="D76" s="15"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="18">
+        <v>43594</v>
+      </c>
+      <c r="J76" s="3"/>
+      <c r="K76" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L76" s="15"/>
+      <c r="M76" s="19"/>
+      <c r="N76" s="17"/>
+    </row>
+    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="18">
+        <v>43595</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="20">
-        <v>42486</v>
-      </c>
-      <c r="J63" s="12"/>
-      <c r="K63" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="L63" s="17"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="O63" s="22">
-        <v>7.3333000000000004</v>
-      </c>
-      <c r="P63" s="21"/>
-    </row>
-    <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="13">
-        <v>42487</v>
-      </c>
-      <c r="B64" s="13"/>
-      <c r="C64" s="19" t="s">
+      <c r="D77" s="15"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="18">
+        <v>43595</v>
+      </c>
+      <c r="J77" s="3"/>
+      <c r="K77" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L77" s="15"/>
+      <c r="M77" s="19"/>
+      <c r="N77" s="17"/>
+    </row>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="18">
+        <v>43596</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="20">
-        <v>42487</v>
-      </c>
-      <c r="J64" s="12"/>
-      <c r="K64" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L64" s="17"/>
-      <c r="M64" s="17"/>
-      <c r="N64" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O64" s="22">
-        <v>6.5</v>
-      </c>
-      <c r="P64" s="21"/>
-    </row>
-    <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="13">
-        <v>42488</v>
-      </c>
-      <c r="B65" s="13"/>
-      <c r="C65" s="19" t="s">
+      <c r="D78" s="15"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="18">
+        <v>43596</v>
+      </c>
+      <c r="J78" s="3"/>
+      <c r="K78" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L78" s="15"/>
+      <c r="M78" s="19"/>
+      <c r="N78" s="17"/>
+    </row>
+    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="18">
+        <v>43597</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="17"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="20">
-        <v>42488</v>
-      </c>
-      <c r="J65" s="12"/>
-      <c r="K65" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L65" s="17"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="23"/>
-      <c r="O65" s="17"/>
-      <c r="P65" s="21"/>
-    </row>
-    <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="13">
-        <v>42489</v>
-      </c>
-      <c r="B66" s="24"/>
-      <c r="C66" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="17"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="20">
-        <v>42489</v>
-      </c>
-      <c r="J66" s="12"/>
-      <c r="K66" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L66" s="17"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="19"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="21"/>
-    </row>
-    <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="13">
-        <v>42490</v>
-      </c>
-      <c r="B67" s="24"/>
-      <c r="C67" s="17" t="s">
+      <c r="D79" s="15"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="18">
+        <v>43597</v>
+      </c>
+      <c r="J79" s="3"/>
+      <c r="K79" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L79" s="15"/>
+      <c r="M79" s="19"/>
+      <c r="N79" s="17"/>
+    </row>
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="18">
+        <v>43598</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E80" s="19"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="18">
+        <v>43598</v>
+      </c>
+      <c r="J80" s="3"/>
+      <c r="K80" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L80" s="15"/>
+      <c r="M80" s="19"/>
+      <c r="N80" s="17"/>
+    </row>
+    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="18">
+        <v>43599</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D67" s="17"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="21"/>
-      <c r="I67" s="13">
-        <v>42490</v>
-      </c>
-      <c r="J67" s="3"/>
-      <c r="K67" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="L67" s="17"/>
-      <c r="M67" s="21"/>
-      <c r="N67" s="17"/>
-      <c r="O67" s="17"/>
-      <c r="P67" s="21"/>
-    </row>
-    <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="13">
-        <v>43586</v>
-      </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="32" t="s">
+      <c r="D81" s="15"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="19"/>
+      <c r="I81" s="18">
+        <v>43599</v>
+      </c>
+      <c r="J81" s="3"/>
+      <c r="K81" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L81" s="15"/>
+      <c r="M81" s="19"/>
+      <c r="N81" s="17"/>
+    </row>
+    <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="18">
+        <v>43600</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D68" s="17"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="21"/>
-      <c r="I68" s="13">
-        <v>43586</v>
-      </c>
-      <c r="J68" s="3"/>
-      <c r="K68" s="32" t="s">
+      <c r="D82" s="15"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="19"/>
+      <c r="I82" s="18">
+        <v>43600</v>
+      </c>
+      <c r="J82" s="3"/>
+      <c r="K82" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="L68" s="17"/>
-      <c r="M68" s="21"/>
-      <c r="N68" s="17"/>
-      <c r="O68" s="17"/>
-      <c r="P68" s="21"/>
-      <c r="Q68" s="12"/>
-    </row>
-    <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="13">
-        <v>43587</v>
-      </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="17"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="20">
-        <v>43587</v>
-      </c>
-      <c r="J69" s="3"/>
-      <c r="K69" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="L69" s="17"/>
-      <c r="M69" s="21"/>
-      <c r="N69" s="19"/>
-      <c r="O69" s="17"/>
-      <c r="P69" s="21"/>
-    </row>
-    <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="20">
-        <v>43588</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="17"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="21"/>
-      <c r="I70" s="20">
-        <v>43588</v>
-      </c>
-      <c r="J70" s="3"/>
-      <c r="K70" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="L70" s="17"/>
-      <c r="M70" s="21"/>
-      <c r="N70" s="19"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="21"/>
-    </row>
-    <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="20">
-        <v>43589</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="17"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="21"/>
-      <c r="I71" s="20">
-        <v>43589</v>
-      </c>
-      <c r="J71" s="3"/>
-      <c r="K71" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="L71" s="17"/>
-      <c r="M71" s="21"/>
-      <c r="N71" s="19"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="21"/>
-    </row>
-    <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="20">
-        <v>43590</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="17"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="21"/>
-      <c r="I72" s="20">
-        <v>43590</v>
-      </c>
-      <c r="J72" s="3"/>
-      <c r="K72" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L72" s="17"/>
-      <c r="M72" s="21"/>
-      <c r="N72" s="19"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="21"/>
-    </row>
-    <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="20">
-        <v>43591</v>
-      </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="17"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="21"/>
-      <c r="I73" s="20">
-        <v>43591</v>
-      </c>
-      <c r="J73" s="3"/>
-      <c r="K73" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L73" s="17"/>
-      <c r="M73" s="21"/>
-      <c r="N73" s="19"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="21"/>
-    </row>
-    <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="20">
-        <v>43592</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D74" s="17"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="21"/>
-      <c r="I74" s="20">
-        <v>43592</v>
-      </c>
-      <c r="J74" s="3"/>
-      <c r="K74" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L74" s="17"/>
-      <c r="M74" s="21"/>
-      <c r="N74" s="19"/>
-      <c r="O74" s="17"/>
-      <c r="P74" s="21"/>
-    </row>
-    <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="20">
-        <v>43593</v>
-      </c>
-      <c r="B75" s="3"/>
-      <c r="C75" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" s="17"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="21"/>
-      <c r="I75" s="20">
-        <v>43593</v>
-      </c>
-      <c r="J75" s="3"/>
-      <c r="K75" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="L75" s="17"/>
-      <c r="M75" s="21"/>
-      <c r="N75" s="19"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="21"/>
-    </row>
-    <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="20">
-        <v>43594</v>
-      </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="17"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="20">
-        <v>43594</v>
-      </c>
-      <c r="J76" s="3"/>
-      <c r="K76" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L76" s="17"/>
-      <c r="M76" s="21"/>
-      <c r="N76" s="19"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="21"/>
-    </row>
-    <row r="77" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="20">
-        <v>43595</v>
-      </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="17"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="21"/>
-      <c r="I77" s="20">
-        <v>43595</v>
-      </c>
-      <c r="J77" s="3"/>
-      <c r="K77" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L77" s="17"/>
-      <c r="M77" s="21"/>
-      <c r="N77" s="19"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="21"/>
-    </row>
-    <row r="78" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="20">
-        <v>43596</v>
-      </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="17"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="21"/>
-      <c r="I78" s="20">
-        <v>43596</v>
-      </c>
-      <c r="J78" s="3"/>
-      <c r="K78" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L78" s="17"/>
-      <c r="M78" s="21"/>
-      <c r="N78" s="19"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="21"/>
-    </row>
-    <row r="79" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="20">
-        <v>43597</v>
-      </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" s="17"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="21"/>
-      <c r="I79" s="20">
-        <v>43597</v>
-      </c>
-      <c r="J79" s="3"/>
-      <c r="K79" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L79" s="17"/>
-      <c r="M79" s="21"/>
-      <c r="N79" s="19"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="21"/>
-    </row>
-    <row r="80" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="20">
-        <v>43598</v>
-      </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E80" s="21"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="21"/>
-      <c r="I80" s="20">
-        <v>43598</v>
-      </c>
-      <c r="J80" s="3"/>
-      <c r="K80" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L80" s="17"/>
-      <c r="M80" s="21"/>
-      <c r="N80" s="19"/>
-      <c r="O80" s="17"/>
-      <c r="P80" s="21"/>
-    </row>
-    <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="20">
-        <v>43599</v>
-      </c>
-      <c r="B81" s="3"/>
-      <c r="C81" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D81" s="17"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="21"/>
-      <c r="I81" s="20">
-        <v>43599</v>
-      </c>
-      <c r="J81" s="3"/>
-      <c r="K81" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L81" s="17"/>
-      <c r="M81" s="21"/>
-      <c r="N81" s="19"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="21"/>
-    </row>
-    <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="20">
-        <v>43600</v>
-      </c>
-      <c r="B82" s="3"/>
-      <c r="C82" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D82" s="17"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="21"/>
-      <c r="I82" s="20">
-        <v>43600</v>
-      </c>
-      <c r="J82" s="3"/>
-      <c r="K82" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="L82" s="17"/>
-      <c r="M82" s="21"/>
-      <c r="N82" s="19"/>
-      <c r="O82" s="17"/>
-      <c r="P82" s="21"/>
-    </row>
-    <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="34"/>
-      <c r="B83" s="34"/>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="34"/>
-      <c r="J83" s="34"/>
-      <c r="K83" s="15"/>
-      <c r="L83" s="15"/>
-      <c r="M83" s="15"/>
-      <c r="N83" s="15"/>
-      <c r="O83" s="15"/>
-      <c r="P83" s="15"/>
-    </row>
-    <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="20"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="12"/>
-      <c r="K84" s="17"/>
-      <c r="L84" s="12"/>
-      <c r="M84" s="12"/>
-      <c r="N84" s="12"/>
-      <c r="O84" s="12">
-        <f>O8+O10+O11+O13+O14+O15+O16+O17+O18+O20+O21+O25+O29+O30+O34+O35+O49+O50+O56+O57+O62+O63+O64</f>
-        <v>135.91663</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="87" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="88" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="89" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="90" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="91" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="92" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="93" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="94" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="19"/>
+      <c r="N82" s="17"/>
+    </row>
+    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="32"/>
+      <c r="B83" s="32"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="32"/>
+      <c r="J83" s="32"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13"/>
+    </row>
+    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="18"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+    </row>
+    <row r="85" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
empty unnec col G
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2022.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2022.xlsx
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -767,10 +767,7 @@
       <c r="F11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="20">
-        <f>7+(40/60)</f>
-        <v>7.666666666666667</v>
-      </c>
+      <c r="G11" s="20"/>
       <c r="H11" s="15"/>
       <c r="I11" s="18">
         <v>42434</v>
@@ -952,9 +949,7 @@
       <c r="F18" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="20">
-        <v>4</v>
-      </c>
+      <c r="G18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="18">
         <v>42441</v>
@@ -1130,10 +1125,7 @@
       <c r="F25" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="15">
-        <f>7+(10/60)</f>
-        <v>7.166666666666667</v>
-      </c>
+      <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="18">
         <v>42448</v>

</xml_diff>

<commit_message>
empty row 80 column D
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2022.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_AKL&LK_2022.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="40">
   <si>
     <t>OMGEKEERD SPUIBEHEER AKL 2022</t>
   </si>
@@ -146,12 +146,6 @@
   </si>
   <si>
     <t>geen spuibeheer hogezoutwaarden</t>
-  </si>
-  <si>
-    <t>niet mogelijk pleziervaar</t>
-  </si>
-  <si>
-    <t>door pleziervaart</t>
   </si>
 </sst>
 </file>
@@ -557,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2464,11 +2458,9 @@
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>41</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D80" s="15"/>
       <c r="E80" s="19"/>
       <c r="F80" s="17"/>
       <c r="G80" s="15"/>

</xml_diff>